<commit_message>
Added to methods section, added BMI variables to spreadsheet, added BMI analysis
</commit_message>
<xml_diff>
--- a/Meta Analysis/LDL Study Summary.xlsx
+++ b/Meta Analysis/LDL Study Summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cody\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cody\Documents\GitHub\PrecisionNutrition\Meta Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A5F23A-A1AB-464C-9ED4-F66EA20FA9FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C17CF5-9E0B-408A-BCDD-D8EDAB10183D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1995" yWindow="2145" windowWidth="30615" windowHeight="17100" xr2:uid="{0AAFB315-195C-354F-968F-54E1873F1AC8}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{0AAFB315-195C-354F-968F-54E1873F1AC8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="81">
   <si>
     <t>Study</t>
   </si>
@@ -198,9 +198,6 @@
     <t>Zajac2014</t>
   </si>
   <si>
-    <t>no baseline weight</t>
-  </si>
-  <si>
     <t>crossover</t>
   </si>
   <si>
@@ -226,16 +223,78 @@
   </si>
   <si>
     <t>completers only/in children</t>
+  </si>
+  <si>
+    <t>Baseline BMI</t>
+  </si>
+  <si>
+    <t>BMI Change</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC3981696/</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC5865541/</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC5329646/</t>
+  </si>
+  <si>
+    <t>no BMI</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC5048014/</t>
+  </si>
+  <si>
+    <t>ncbi.nlm.nih.gov/pmc/articles/PMC2633336/</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC2845587/</t>
+  </si>
+  <si>
+    <t>https://pubmed.ncbi.nlm.nih.gov/23155696/</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC6950598/</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC2633336/</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC8001988/#app1-nutrients-13-00814</t>
+  </si>
+  <si>
+    <t>BMI baseline, no endpoint, given as median</t>
+  </si>
+  <si>
+    <t>https://www-sciencedirect-com.proxy.lib.umich.edu/science/article/pii/S0021915018314321</t>
+  </si>
+  <si>
+    <t>No endpoint BMI</t>
+  </si>
+  <si>
+    <t>no baseline weight, no BMI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -258,13 +317,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -577,10 +639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{269637A6-0EDF-4343-81B3-3C675D3434A6}">
-  <dimension ref="A1:P30"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -588,14 +650,15 @@
     <col min="1" max="1" width="15.875" customWidth="1"/>
     <col min="2" max="2" width="14.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.125" customWidth="1"/>
+    <col min="4" max="5" width="13.625" customWidth="1"/>
+    <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.125" customWidth="1"/>
-    <col min="9" max="9" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.125" customWidth="1"/>
+    <col min="11" max="11" width="14.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -606,46 +669,55 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>26</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>20</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>27</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>19</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>16</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>37</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>38</v>
       </c>
-      <c r="P1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R1" t="s">
+        <v>61</v>
+      </c>
+      <c r="S1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -656,34 +728,43 @@
         <v>-5.5</v>
       </c>
       <c r="D2">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="E2">
+        <v>-1.9</v>
+      </c>
+      <c r="F2">
         <v>89.2</v>
       </c>
-      <c r="E2">
+      <c r="G2">
         <v>-2.1</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>25.8</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>33.6</v>
       </c>
-      <c r="J2">
+      <c r="L2">
         <v>16</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>12</v>
       </c>
-      <c r="M2">
+      <c r="O2">
         <v>21</v>
       </c>
-      <c r="O2" t="s">
-        <v>39</v>
-      </c>
-      <c r="P2">
+      <c r="Q2" t="s">
+        <v>39</v>
+      </c>
+      <c r="R2">
         <v>0.437</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -695,35 +776,44 @@
         <v>-6.1000000000000085</v>
       </c>
       <c r="D3">
+        <v>35.9</v>
+      </c>
+      <c r="E3">
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="F3">
         <v>88.7</v>
       </c>
-      <c r="E3">
+      <c r="G3">
         <f>97.9-88.7</f>
         <v>9.2000000000000028</v>
       </c>
-      <c r="F3">
-        <f>SQRT(J3)*H3/3.92</f>
+      <c r="H3">
+        <f>SQRT(L3)*J3/3.92</f>
         <v>12.653061224489797</v>
       </c>
-      <c r="G3">
-        <f>SQRT(J3)*I3/3.92</f>
+      <c r="I3">
+        <f>SQRT(L3)*K3/3.92</f>
         <v>12.857142857142852</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>12.4</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <f>110.5-97.9</f>
         <v>12.599999999999994</v>
       </c>
-      <c r="J3">
+      <c r="L3">
         <v>16</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -735,41 +825,50 @@
         <v>-7.9000000000000057</v>
       </c>
       <c r="D4">
+        <v>35.9</v>
+      </c>
+      <c r="E4">
+        <v>-2.6</v>
+      </c>
+      <c r="F4">
         <v>88.7</v>
       </c>
-      <c r="E4">
+      <c r="G4">
         <f>95.6-88.7</f>
         <v>6.8999999999999915</v>
       </c>
-      <c r="F4">
-        <f>SQRT(J4)*H4/3.92</f>
+      <c r="H4">
+        <f>SQRT(L4)*J4/3.92</f>
         <v>12.653061224489797</v>
       </c>
-      <c r="G4">
-        <f>SQRT(J4)*I4/3.92</f>
+      <c r="I4">
+        <f>SQRT(L4)*K4/3.92</f>
         <v>13.571428571428584</v>
       </c>
-      <c r="H4">
+      <c r="J4">
         <v>12.4</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <f>108.9-95.6</f>
         <v>13.300000000000011</v>
       </c>
-      <c r="J4">
+      <c r="L4">
         <v>16</v>
       </c>
-      <c r="K4" t="s">
+      <c r="M4" t="s">
         <v>10</v>
       </c>
-      <c r="O4" t="s">
-        <v>39</v>
-      </c>
-      <c r="P4">
+      <c r="Q4" t="s">
+        <v>39</v>
+      </c>
+      <c r="R4">
         <v>0.11</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -779,26 +878,32 @@
       <c r="C5">
         <v>-8.5</v>
       </c>
-      <c r="D5">
+      <c r="F5">
         <v>96.9</v>
       </c>
-      <c r="E5">
+      <c r="G5">
         <v>-0.8</v>
       </c>
-      <c r="F5">
+      <c r="H5">
         <v>30.4</v>
       </c>
-      <c r="J5">
+      <c r="L5">
         <v>12</v>
       </c>
-      <c r="K5" t="s">
+      <c r="M5" t="s">
         <v>14</v>
       </c>
-      <c r="L5">
+      <c r="N5">
         <v>10.1</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P5" t="s">
+        <v>69</v>
+      </c>
+      <c r="S5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -808,32 +913,38 @@
       <c r="C6">
         <v>-12.7</v>
       </c>
-      <c r="D6">
+      <c r="F6">
         <v>96.9</v>
       </c>
-      <c r="E6">
+      <c r="G6">
         <v>-0.3</v>
       </c>
-      <c r="F6">
+      <c r="H6">
         <v>30.4</v>
       </c>
-      <c r="J6">
+      <c r="L6">
         <v>12</v>
       </c>
-      <c r="K6" t="s">
+      <c r="M6" t="s">
         <v>15</v>
       </c>
-      <c r="L6">
+      <c r="N6">
         <v>10.5</v>
       </c>
-      <c r="O6" t="s">
-        <v>39</v>
-      </c>
-      <c r="P6">
+      <c r="P6" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>39</v>
+      </c>
+      <c r="R6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -845,40 +956,49 @@
         <v>-14.670000000000002</v>
       </c>
       <c r="D7">
+        <v>33.25</v>
+      </c>
+      <c r="E7">
+        <v>-5.4</v>
+      </c>
+      <c r="F7">
         <v>112.7</v>
       </c>
-      <c r="E7">
+      <c r="G7">
         <f>110.6-112.7</f>
         <v>-2.1000000000000085</v>
       </c>
-      <c r="F7">
+      <c r="H7">
         <v>33.6</v>
       </c>
-      <c r="G7">
+      <c r="I7">
         <v>38.4</v>
       </c>
-      <c r="J7">
+      <c r="L7">
         <v>45</v>
       </c>
-      <c r="K7" t="s">
+      <c r="M7" t="s">
         <v>18</v>
       </c>
-      <c r="O7" t="s">
-        <v>39</v>
-      </c>
-      <c r="P7">
+      <c r="Q7" t="s">
+        <v>39</v>
+      </c>
+      <c r="R7">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
-      <c r="N8" t="s">
+      <c r="P8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -889,17 +1009,17 @@
         <f>100.1-108.4</f>
         <v>-8.3000000000000114</v>
       </c>
-      <c r="D9">
+      <c r="F9">
         <v>107.1</v>
       </c>
-      <c r="J9">
+      <c r="L9">
         <v>21</v>
       </c>
-      <c r="K9" t="s">
+      <c r="M9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -911,32 +1031,41 @@
         <v>-11.100000000000009</v>
       </c>
       <c r="D10">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="E10">
+        <v>-3.9</v>
+      </c>
+      <c r="F10">
         <v>105.8</v>
       </c>
-      <c r="E10">
+      <c r="G10">
         <f>107.1-105.8</f>
         <v>1.2999999999999972</v>
       </c>
-      <c r="F10">
+      <c r="H10">
         <v>25.7</v>
       </c>
-      <c r="G10">
+      <c r="I10">
         <v>26.3</v>
       </c>
-      <c r="J10">
+      <c r="L10">
         <v>21</v>
       </c>
-      <c r="K10" t="s">
+      <c r="M10" t="s">
         <v>25</v>
       </c>
-      <c r="O10" t="s">
-        <v>39</v>
-      </c>
-      <c r="P10">
+      <c r="Q10" t="s">
+        <v>39</v>
+      </c>
+      <c r="R10">
         <v>0.33300000000000002</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -947,39 +1076,48 @@
         <v>-5.6</v>
       </c>
       <c r="D11">
+        <v>32.9</v>
+      </c>
+      <c r="E11">
+        <v>-1.9</v>
+      </c>
+      <c r="F11">
         <f>3.3*38.76</f>
         <v>127.90799999999999</v>
       </c>
-      <c r="E11">
-        <f>3.5*38.76-D11</f>
+      <c r="G11">
+        <f>3.5*38.76-F11</f>
         <v>7.7520000000000095</v>
       </c>
-      <c r="F11">
+      <c r="H11">
         <f>0.9*38.76</f>
         <v>34.884</v>
       </c>
-      <c r="G11">
+      <c r="I11">
         <f>1.1*38.76</f>
         <v>42.636000000000003</v>
       </c>
-      <c r="J11">
+      <c r="L11">
         <v>16</v>
       </c>
-      <c r="K11" t="s">
+      <c r="M11" t="s">
         <v>29</v>
       </c>
-      <c r="M11">
+      <c r="O11">
         <f>0.9*38.76</f>
         <v>34.884</v>
       </c>
-      <c r="O11" t="s">
-        <v>39</v>
-      </c>
-      <c r="P11">
+      <c r="Q11" t="s">
+        <v>39</v>
+      </c>
+      <c r="R11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -991,38 +1129,47 @@
         <v>-8</v>
       </c>
       <c r="D12">
+        <v>30.8</v>
+      </c>
+      <c r="E12">
+        <v>-0.8</v>
+      </c>
+      <c r="F12">
         <f>2.72*38.76</f>
         <v>105.4272</v>
       </c>
-      <c r="E12">
-        <f>2.86*38.76-D12</f>
+      <c r="G12">
+        <f>2.86*38.76-F12</f>
         <v>5.4263999999999868</v>
       </c>
-      <c r="F12">
+      <c r="H12">
         <f>0.69*38.76</f>
         <v>26.744399999999995</v>
       </c>
-      <c r="G12">
+      <c r="I12">
         <f>0.65*38.76</f>
         <v>25.193999999999999</v>
       </c>
-      <c r="J12">
+      <c r="L12">
         <v>21</v>
       </c>
-      <c r="K12" t="s">
+      <c r="M12" t="s">
         <v>9</v>
       </c>
-      <c r="N12" t="s">
-        <v>63</v>
-      </c>
-      <c r="O12" t="s">
-        <v>39</v>
-      </c>
-      <c r="P12">
+      <c r="P12" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>39</v>
+      </c>
+      <c r="R12">
         <v>0.48</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S12" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -1034,42 +1181,51 @@
         <v>-2.7999999999999972</v>
       </c>
       <c r="D13">
+        <v>25</v>
+      </c>
+      <c r="E13">
+        <v>-1</v>
+      </c>
+      <c r="F13">
         <f>3.3*38.76</f>
         <v>127.90799999999999</v>
       </c>
-      <c r="E13">
-        <f>(4.2*38.76)-D13</f>
+      <c r="G13">
+        <f>(4.2*38.76)-F13</f>
         <v>34.884000000000015</v>
       </c>
-      <c r="F13">
+      <c r="H13">
         <f>1*38.76</f>
         <v>38.76</v>
       </c>
-      <c r="G13">
+      <c r="I13">
         <f>1.2*38.76</f>
         <v>46.511999999999993</v>
       </c>
-      <c r="J13">
+      <c r="L13">
         <v>20</v>
       </c>
-      <c r="K13" t="s">
+      <c r="M13" t="s">
         <v>42</v>
       </c>
-      <c r="M13">
+      <c r="O13">
         <f>0.98*38.76</f>
         <v>37.9848</v>
       </c>
-      <c r="N13" t="s">
+      <c r="P13" t="s">
         <v>33</v>
       </c>
-      <c r="O13" t="s">
-        <v>39</v>
-      </c>
-      <c r="P13">
+      <c r="Q13" t="s">
+        <v>39</v>
+      </c>
+      <c r="R13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -1079,29 +1235,29 @@
       <c r="C14">
         <v>-9.68</v>
       </c>
-      <c r="D14">
+      <c r="F14">
         <v>151.9</v>
       </c>
-      <c r="E14">
+      <c r="G14">
         <v>3.12</v>
       </c>
-      <c r="F14">
+      <c r="H14">
         <v>74.3</v>
       </c>
-      <c r="J14">
+      <c r="L14">
         <v>57</v>
       </c>
-      <c r="K14" t="s">
+      <c r="M14" t="s">
         <v>24</v>
       </c>
-      <c r="N14" t="s">
+      <c r="P14" t="s">
         <v>31</v>
       </c>
-      <c r="P14">
+      <c r="R14">
         <v>0.75</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -1112,28 +1268,37 @@
         <v>-12.81</v>
       </c>
       <c r="D15">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="E15">
+        <v>-3.9</v>
+      </c>
+      <c r="F15">
         <v>151.9</v>
       </c>
-      <c r="E15">
+      <c r="G15">
         <v>8.09</v>
       </c>
-      <c r="F15">
+      <c r="H15">
         <v>74.3</v>
       </c>
-      <c r="J15">
+      <c r="L15">
         <v>57</v>
       </c>
-      <c r="K15" t="s">
+      <c r="M15" t="s">
         <v>25</v>
       </c>
-      <c r="O15" t="s">
-        <v>39</v>
-      </c>
-      <c r="P15">
+      <c r="Q15" t="s">
+        <v>39</v>
+      </c>
+      <c r="R15">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -1143,26 +1308,26 @@
       <c r="C16">
         <v>-12.38</v>
       </c>
-      <c r="D16">
+      <c r="F16">
         <v>151.9</v>
       </c>
-      <c r="E16">
+      <c r="G16">
         <v>3.19</v>
       </c>
-      <c r="F16">
+      <c r="H16">
         <v>74.3</v>
       </c>
-      <c r="J16">
+      <c r="L16">
         <v>57</v>
       </c>
-      <c r="K16" t="s">
+      <c r="M16" t="s">
         <v>35</v>
       </c>
-      <c r="P16">
+      <c r="R16">
         <v>0.75</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -1172,69 +1337,72 @@
       <c r="C17">
         <v>-11.37</v>
       </c>
-      <c r="D17">
+      <c r="F17">
         <v>151.9</v>
       </c>
-      <c r="E17">
+      <c r="G17">
         <v>-19.100000000000001</v>
       </c>
-      <c r="F17">
+      <c r="H17">
         <v>74.3</v>
       </c>
-      <c r="J17">
+      <c r="L17">
         <v>57</v>
       </c>
-      <c r="K17" t="s">
+      <c r="M17" t="s">
         <v>36</v>
       </c>
-      <c r="P17">
+      <c r="R17">
         <v>0.75</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>41</v>
       </c>
       <c r="B18">
         <v>60.8</v>
       </c>
-      <c r="D18">
+      <c r="F18">
         <f>2.1*38.76</f>
         <v>81.396000000000001</v>
       </c>
-      <c r="E18">
+      <c r="G18">
         <f>1.82*38.76</f>
         <v>70.543199999999999</v>
       </c>
-      <c r="F18">
+      <c r="H18">
         <f>0.6*38.76</f>
         <v>23.255999999999997</v>
       </c>
-      <c r="G18">
-        <f>SQRT(J18)*I18/3.92</f>
+      <c r="I18">
+        <f>SQRT(L18)*K18/3.92</f>
         <v>16.908061224489796</v>
       </c>
-      <c r="I18">
+      <c r="K18">
         <f>(2.39-1.82)*38.76</f>
         <v>22.0932</v>
       </c>
-      <c r="J18">
+      <c r="L18">
         <v>9</v>
       </c>
-      <c r="K18" t="s">
+      <c r="M18" t="s">
         <v>42</v>
       </c>
-      <c r="N18" t="s">
+      <c r="P18" t="s">
         <v>43</v>
       </c>
-      <c r="O18" t="s">
-        <v>39</v>
-      </c>
-      <c r="P18">
+      <c r="Q18" t="s">
+        <v>39</v>
+      </c>
+      <c r="R18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>44</v>
       </c>
@@ -1245,27 +1413,30 @@
         <f>71.4-73.7</f>
         <v>-2.2999999999999972</v>
       </c>
-      <c r="D19">
+      <c r="F19">
         <v>116</v>
       </c>
-      <c r="E19">
+      <c r="G19">
         <f>157-116</f>
         <v>41</v>
       </c>
-      <c r="J19">
+      <c r="L19">
         <v>12</v>
       </c>
-      <c r="K19" t="s">
+      <c r="M19" t="s">
         <v>45</v>
       </c>
-      <c r="O19" t="s">
-        <v>39</v>
-      </c>
-      <c r="P19">
+      <c r="P19" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>39</v>
+      </c>
+      <c r="R19">
         <v>0.58299999999999996</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>46</v>
       </c>
@@ -1277,35 +1448,44 @@
         <v>-1.2000000000000028</v>
       </c>
       <c r="D20">
+        <v>21.7</v>
+      </c>
+      <c r="E20">
+        <v>-0.4</v>
+      </c>
+      <c r="F20">
         <f>2.2*38.76</f>
         <v>85.272000000000006</v>
       </c>
-      <c r="E20">
-        <f>3.1*38.76-D20</f>
+      <c r="G20">
+        <f>3.1*38.76-F20</f>
         <v>34.883999999999986</v>
       </c>
-      <c r="F20">
+      <c r="H20">
         <f>0.4*38.76</f>
         <v>15.504</v>
       </c>
-      <c r="G20">
+      <c r="I20">
         <f>0.8*38.76</f>
         <v>31.007999999999999</v>
       </c>
-      <c r="J20">
+      <c r="L20">
         <v>15</v>
       </c>
-      <c r="K20" t="s">
+      <c r="M20" t="s">
         <v>47</v>
       </c>
-      <c r="O20" t="s">
-        <v>39</v>
-      </c>
-      <c r="P20">
+      <c r="Q20" t="s">
+        <v>39</v>
+      </c>
+      <c r="R20">
         <v>6.7000000000000004E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>48</v>
       </c>
@@ -1317,32 +1497,38 @@
         <v>-1.8999999999999915</v>
       </c>
       <c r="D21">
+        <v>23.9</v>
+      </c>
+      <c r="F21">
         <v>110.9</v>
       </c>
-      <c r="E21">
-        <f>122.8-D21</f>
+      <c r="G21">
+        <f>122.8-F21</f>
         <v>11.899999999999991</v>
       </c>
-      <c r="F21">
+      <c r="H21">
         <v>31.3</v>
       </c>
-      <c r="G21">
+      <c r="I21">
         <v>33.6</v>
       </c>
-      <c r="J21">
+      <c r="L21">
         <v>42</v>
       </c>
-      <c r="K21" t="s">
+      <c r="M21" t="s">
         <v>49</v>
       </c>
-      <c r="O21" t="s">
-        <v>39</v>
-      </c>
-      <c r="P21">
+      <c r="P21" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>39</v>
+      </c>
+      <c r="R21">
         <v>0.26200000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>50</v>
       </c>
@@ -1353,75 +1539,75 @@
         <f>73.3-73.8</f>
         <v>-0.5</v>
       </c>
-      <c r="D22">
+      <c r="F22">
         <f>159-40</f>
         <v>119</v>
       </c>
-      <c r="E22">
-        <f>(208-40)-D22</f>
+      <c r="G22">
+        <f>(208-40)-F22</f>
         <v>49</v>
       </c>
-      <c r="F22">
+      <c r="H22">
         <f>SQRT(9^2+4.4^2)</f>
         <v>10.017983829094554</v>
       </c>
-      <c r="G22">
+      <c r="I22">
         <f>SQRT(7.7^2+1^2)</f>
         <v>7.7646635471216658</v>
       </c>
-      <c r="J22">
+      <c r="L22">
         <v>9</v>
       </c>
-      <c r="K22" t="s">
+      <c r="M22" t="s">
         <v>42</v>
       </c>
-      <c r="N22" t="s">
+      <c r="P22" t="s">
         <v>51</v>
       </c>
-      <c r="P22">
+      <c r="R22">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>52</v>
       </c>
       <c r="C23">
         <v>-2.2000000000000002</v>
       </c>
-      <c r="D23">
+      <c r="F23">
         <f>2.87*38.76</f>
         <v>111.24119999999999</v>
       </c>
-      <c r="E23">
-        <f>2.99*38.76-D23</f>
+      <c r="G23">
+        <f>2.99*38.76-F23</f>
         <v>4.6512000000000171</v>
       </c>
-      <c r="F23">
+      <c r="H23">
         <f>0.8*38.76</f>
         <v>31.007999999999999</v>
       </c>
-      <c r="G23">
+      <c r="I23">
         <f>0.8*38.76</f>
         <v>31.007999999999999</v>
       </c>
-      <c r="J23">
+      <c r="L23">
         <v>12</v>
       </c>
-      <c r="K23" t="s">
+      <c r="M23" t="s">
         <v>49</v>
       </c>
-      <c r="N23" t="s">
-        <v>54</v>
-      </c>
-      <c r="O23" t="s">
-        <v>39</v>
-      </c>
-      <c r="P23">
+      <c r="P23" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>39</v>
+      </c>
+      <c r="R23">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>53</v>
       </c>
@@ -1433,69 +1619,75 @@
         <v>-2.0799999999999983</v>
       </c>
       <c r="D24">
+        <v>24.9</v>
+      </c>
+      <c r="E24">
+        <v>-1</v>
+      </c>
+      <c r="F24">
         <v>64.12</v>
       </c>
-      <c r="E24">
+      <c r="G24">
         <f>74.8-64.12</f>
         <v>10.679999999999993</v>
       </c>
-      <c r="F24">
+      <c r="H24">
         <v>4.21</v>
       </c>
-      <c r="G24">
+      <c r="I24">
         <v>5.12</v>
       </c>
-      <c r="J24">
+      <c r="L24">
         <v>8</v>
       </c>
-      <c r="K24" t="s">
+      <c r="M24" t="s">
         <v>42</v>
       </c>
-      <c r="N24" t="s">
-        <v>55</v>
-      </c>
-      <c r="O24" t="s">
-        <v>39</v>
-      </c>
-      <c r="P24">
+      <c r="P24" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>39</v>
+      </c>
+      <c r="R24">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C25">
         <v>-5.4</v>
       </c>
-      <c r="D25">
+      <c r="F25">
         <v>165.6</v>
       </c>
-      <c r="E25">
+      <c r="G25">
         <v>-2.2000000000000002</v>
       </c>
-      <c r="F25">
+      <c r="H25">
         <v>39.700000000000003</v>
       </c>
-      <c r="G25">
+      <c r="I25">
         <v>19.3</v>
       </c>
-      <c r="J25">
-        <v>39</v>
-      </c>
-      <c r="K25" t="s">
+      <c r="L25">
+        <v>39</v>
+      </c>
+      <c r="M25" t="s">
         <v>49</v>
       </c>
-      <c r="O25" t="s">
-        <v>39</v>
-      </c>
-      <c r="P25">
+      <c r="Q25" t="s">
+        <v>39</v>
+      </c>
+      <c r="R25">
         <v>0.39</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B26">
         <v>114</v>
@@ -1503,38 +1695,38 @@
       <c r="C26">
         <v>-3.8</v>
       </c>
-      <c r="D26">
+      <c r="F26">
         <v>122</v>
       </c>
-      <c r="E26">
+      <c r="G26">
         <v>-4</v>
       </c>
-      <c r="F26">
+      <c r="H26">
         <v>26</v>
       </c>
-      <c r="G26">
+      <c r="I26">
         <v>35</v>
       </c>
-      <c r="J26">
+      <c r="L26">
         <v>16</v>
       </c>
-      <c r="K26" t="s">
+      <c r="M26" t="s">
         <v>47</v>
       </c>
-      <c r="N26" t="s">
-        <v>55</v>
-      </c>
-      <c r="O26" t="s">
-        <v>39</v>
-      </c>
-      <c r="P26">
+      <c r="P26" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>39</v>
+      </c>
+      <c r="R26">
         <f>10/16</f>
         <v>0.625</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B27">
         <v>109.1</v>
@@ -1542,34 +1734,34 @@
       <c r="C27">
         <v>-6.1</v>
       </c>
-      <c r="D27">
+      <c r="F27">
         <v>125.4</v>
       </c>
-      <c r="E27">
+      <c r="G27">
         <v>-7.7</v>
       </c>
-      <c r="F27">
+      <c r="H27">
         <v>28.2</v>
       </c>
-      <c r="G27">
+      <c r="I27">
         <v>30.9</v>
       </c>
-      <c r="J27">
+      <c r="L27">
         <v>15</v>
       </c>
-      <c r="K27" t="s">
+      <c r="M27" t="s">
         <v>49</v>
       </c>
-      <c r="O27" t="s">
-        <v>39</v>
-      </c>
-      <c r="P27">
+      <c r="Q27" t="s">
+        <v>39</v>
+      </c>
+      <c r="R27">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B28">
         <v>59.8</v>
@@ -1577,34 +1769,34 @@
       <c r="C28">
         <v>0</v>
       </c>
-      <c r="D28">
+      <c r="F28">
         <v>113.5</v>
       </c>
-      <c r="E28">
+      <c r="G28">
         <v>16.600000000000001</v>
       </c>
-      <c r="F28">
+      <c r="H28">
         <v>34</v>
       </c>
-      <c r="G28">
+      <c r="I28">
         <v>23.9</v>
       </c>
-      <c r="J28">
+      <c r="L28">
         <v>10</v>
       </c>
-      <c r="K28" t="s">
+      <c r="M28" t="s">
         <v>42</v>
       </c>
-      <c r="O28" t="s">
-        <v>39</v>
-      </c>
-      <c r="P28">
+      <c r="Q28" t="s">
+        <v>39</v>
+      </c>
+      <c r="R28">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B29">
         <v>76.2</v>
@@ -1612,68 +1804,77 @@
       <c r="C29">
         <v>-2.96</v>
       </c>
-      <c r="D29">
+      <c r="F29">
         <v>113</v>
       </c>
-      <c r="E29">
+      <c r="G29">
         <v>6</v>
       </c>
-      <c r="F29">
+      <c r="H29">
         <v>30</v>
       </c>
-      <c r="G29">
+      <c r="I29">
         <v>29</v>
       </c>
-      <c r="J29">
+      <c r="L29">
         <v>13</v>
       </c>
-      <c r="K29" t="s">
+      <c r="M29" t="s">
         <v>42</v>
       </c>
-      <c r="O29" t="s">
-        <v>39</v>
-      </c>
-      <c r="P29">
+      <c r="Q29" t="s">
+        <v>39</v>
+      </c>
+      <c r="R29">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B30">
-        <v>96.5</v>
+        <v>94.4</v>
       </c>
       <c r="C30">
-        <v>-10.1</v>
+        <v>-5.2</v>
       </c>
       <c r="D30">
-        <v>130</v>
+        <v>32.1</v>
       </c>
       <c r="E30">
-        <v>5</v>
+        <v>-1.8</v>
       </c>
       <c r="F30">
-        <v>22</v>
+        <v>128</v>
       </c>
       <c r="G30">
+        <v>-2</v>
+      </c>
+      <c r="H30">
         <v>31</v>
       </c>
-      <c r="J30">
-        <v>40</v>
-      </c>
-      <c r="K30" t="s">
+      <c r="I30">
+        <v>32</v>
+      </c>
+      <c r="L30">
+        <v>20</v>
+      </c>
+      <c r="M30" t="s">
         <v>24</v>
       </c>
-      <c r="O30" t="s">
-        <v>39</v>
-      </c>
-      <c r="P30">
+      <c r="Q30" t="s">
+        <v>39</v>
+      </c>
+      <c r="R30">
         <v>0.5</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="S12" r:id="rId1" xr:uid="{DF393319-4305-403F-8ADC-047B02A02027}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added 2 studies to summary excel sheet
</commit_message>
<xml_diff>
--- a/Meta Analysis/LDL Study Summary.xlsx
+++ b/Meta Analysis/LDL Study Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cody\Documents\GitHub\PrecisionNutrition\Meta Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C17CF5-9E0B-408A-BCDD-D8EDAB10183D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA4462A4-6E01-4498-9EE3-A5BCBB82015E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{0AAFB315-195C-354F-968F-54E1873F1AC8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{0AAFB315-195C-354F-968F-54E1873F1AC8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="88">
   <si>
     <t>Study</t>
   </si>
@@ -277,6 +277,27 @@
   </si>
   <si>
     <t>no baseline weight, no BMI</t>
+  </si>
+  <si>
+    <t>DAlessio2003</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/jcem/article/88/4/1617/2845298?login=false</t>
+  </si>
+  <si>
+    <t>CHO too high</t>
+  </si>
+  <si>
+    <t>Klein2003</t>
+  </si>
+  <si>
+    <t>Klein2003b</t>
+  </si>
+  <si>
+    <t>Cannot find actual macro intake, individuals instructed to eat less than 20 g CHO/day to start</t>
+  </si>
+  <si>
+    <t>https://www.nejm.org/doi/10.1056/NEJMoa022207?url_ver=Z39.88-2003&amp;rfr_id=ori:rid:crossref.org&amp;rfr_dat=cr_pub%20%200www.ncbi.nlm.nih.gov</t>
   </si>
 </sst>
 </file>
@@ -639,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{269637A6-0EDF-4343-81B3-3C675D3434A6}">
-  <dimension ref="A1:S30"/>
+  <dimension ref="A1:S34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="S39" sqref="S39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1870,11 +1891,161 @@
         <v>0.5</v>
       </c>
     </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>81</v>
+      </c>
+      <c r="B31">
+        <v>91.2</v>
+      </c>
+      <c r="C31">
+        <v>-7.6</v>
+      </c>
+      <c r="D31">
+        <v>33.17</v>
+      </c>
+      <c r="F31">
+        <v>124.86</v>
+      </c>
+      <c r="G31">
+        <v>-11.86</v>
+      </c>
+      <c r="H31">
+        <v>5.39</v>
+      </c>
+      <c r="I31">
+        <v>5.34</v>
+      </c>
+      <c r="L31">
+        <v>22</v>
+      </c>
+      <c r="M31" t="s">
+        <v>12</v>
+      </c>
+      <c r="P31" t="s">
+        <v>83</v>
+      </c>
+      <c r="S31" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>81</v>
+      </c>
+      <c r="B32">
+        <v>91.2</v>
+      </c>
+      <c r="C32">
+        <v>-8.5</v>
+      </c>
+      <c r="D32">
+        <v>33.17</v>
+      </c>
+      <c r="F32">
+        <v>124.86</v>
+      </c>
+      <c r="G32">
+        <v>-0.86</v>
+      </c>
+      <c r="H32">
+        <v>5.39</v>
+      </c>
+      <c r="I32">
+        <v>5.81</v>
+      </c>
+      <c r="L32">
+        <v>22</v>
+      </c>
+      <c r="M32" t="s">
+        <v>9</v>
+      </c>
+      <c r="P32" t="s">
+        <v>83</v>
+      </c>
+      <c r="S32" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>84</v>
+      </c>
+      <c r="B33">
+        <v>98.7</v>
+      </c>
+      <c r="C33">
+        <v>-6.7</v>
+      </c>
+      <c r="D33">
+        <v>33.9</v>
+      </c>
+      <c r="F33">
+        <v>129.5</v>
+      </c>
+      <c r="G33">
+        <v>7</v>
+      </c>
+      <c r="H33">
+        <v>30</v>
+      </c>
+      <c r="I33">
+        <v>19.2</v>
+      </c>
+      <c r="L33">
+        <v>33</v>
+      </c>
+      <c r="M33" t="s">
+        <v>12</v>
+      </c>
+      <c r="P33" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>39</v>
+      </c>
+      <c r="S33" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>85</v>
+      </c>
+      <c r="B34">
+        <v>98.7</v>
+      </c>
+      <c r="C34">
+        <v>-6.9</v>
+      </c>
+      <c r="D34">
+        <v>33.9</v>
+      </c>
+      <c r="F34">
+        <v>129.5</v>
+      </c>
+      <c r="G34">
+        <v>3.5</v>
+      </c>
+      <c r="H34">
+        <v>30</v>
+      </c>
+      <c r="I34">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="L34">
+        <v>33</v>
+      </c>
+      <c r="M34" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="S12" r:id="rId1" xr:uid="{DF393319-4305-403F-8ADC-047B02A02027}"/>
+    <hyperlink ref="S32" r:id="rId2" xr:uid="{F8949122-1CA4-4C9A-9926-43CC41147D5D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added new data to dataset, updated graph and added new models for BMI/LDL
</commit_message>
<xml_diff>
--- a/Meta Analysis/LDL Study Summary.xlsx
+++ b/Meta Analysis/LDL Study Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cody\Documents\GitHub\PrecisionNutrition\Meta Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA4462A4-6E01-4498-9EE3-A5BCBB82015E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09279B37-C1F4-465F-B568-FBB9699B0324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{0AAFB315-195C-354F-968F-54E1873F1AC8}"/>
   </bookViews>
@@ -663,7 +663,7 @@
   <dimension ref="A1:S34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S39" sqref="S39"/>
+      <selection activeCell="R34" sqref="R34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2004,7 +2004,10 @@
       <c r="Q33" t="s">
         <v>39</v>
       </c>
-      <c r="S33" t="s">
+      <c r="R33">
+        <v>0.36</v>
+      </c>
+      <c r="S33" s="1" t="s">
         <v>87</v>
       </c>
     </row>
@@ -2044,8 +2047,9 @@
   <hyperlinks>
     <hyperlink ref="S12" r:id="rId1" xr:uid="{DF393319-4305-403F-8ADC-047B02A02027}"/>
     <hyperlink ref="S32" r:id="rId2" xr:uid="{F8949122-1CA4-4C9A-9926-43CC41147D5D}"/>
+    <hyperlink ref="S33" r:id="rId3" xr:uid="{BFEA82BC-0F1A-4FE2-9C30-7C5358E0CE80}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added a normal weight category to spreadsheet, updated models
</commit_message>
<xml_diff>
--- a/Meta Analysis/LDL Study Summary.xlsx
+++ b/Meta Analysis/LDL Study Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cody\Documents\GitHub\PrecisionNutrition\Meta Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09279B37-C1F4-465F-B568-FBB9699B0324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{832DFC19-5CA9-47F0-96DF-54DE9B422C70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{0AAFB315-195C-354F-968F-54E1873F1AC8}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="91">
   <si>
     <t>Study</t>
   </si>
@@ -298,6 +298,15 @@
   </si>
   <si>
     <t>https://www.nejm.org/doi/10.1056/NEJMoa022207?url_ver=Z39.88-2003&amp;rfr_id=ori:rid:crossref.org&amp;rfr_dat=cr_pub%20%200www.ncbi.nlm.nih.gov</t>
+  </si>
+  <si>
+    <t>Normal weight</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -660,10 +669,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{269637A6-0EDF-4343-81B3-3C675D3434A6}">
-  <dimension ref="A1:S34"/>
+  <dimension ref="A1:T34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R34" sqref="R34"/>
+      <selection activeCell="T39" sqref="T39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -679,7 +688,7 @@
     <col min="11" max="11" width="14.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -735,10 +744,13 @@
         <v>61</v>
       </c>
       <c r="S1" t="s">
+        <v>88</v>
+      </c>
+      <c r="T1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -782,10 +794,13 @@
         <v>0.437</v>
       </c>
       <c r="S2" t="s">
+        <v>89</v>
+      </c>
+      <c r="T2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -831,10 +846,13 @@
         <v>9</v>
       </c>
       <c r="S3" t="s">
+        <v>89</v>
+      </c>
+      <c r="T3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -886,10 +904,13 @@
         <v>0.11</v>
       </c>
       <c r="S4" t="s">
+        <v>89</v>
+      </c>
+      <c r="T4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -920,11 +941,11 @@
       <c r="P5" t="s">
         <v>69</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -961,11 +982,11 @@
       <c r="R6">
         <v>0.5</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1008,10 +1029,13 @@
         <v>0.33</v>
       </c>
       <c r="S7" t="s">
+        <v>89</v>
+      </c>
+      <c r="T7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1019,7 +1043,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1040,7 +1064,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1083,10 +1107,13 @@
         <v>0.33300000000000002</v>
       </c>
       <c r="S10" t="s">
+        <v>89</v>
+      </c>
+      <c r="T10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -1135,10 +1162,13 @@
         <v>0</v>
       </c>
       <c r="S11" t="s">
+        <v>89</v>
+      </c>
+      <c r="T11" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -1186,11 +1216,14 @@
       <c r="R12">
         <v>0.48</v>
       </c>
-      <c r="S12" s="1" t="s">
+      <c r="S12" t="s">
+        <v>89</v>
+      </c>
+      <c r="T12" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -1243,10 +1276,13 @@
         <v>0</v>
       </c>
       <c r="S13" t="s">
+        <v>90</v>
+      </c>
+      <c r="T13" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -1278,7 +1314,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -1316,10 +1352,13 @@
         <v>0.75</v>
       </c>
       <c r="S15" t="s">
+        <v>89</v>
+      </c>
+      <c r="T15" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -1348,7 +1387,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -1377,7 +1416,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -1419,11 +1458,11 @@
       <c r="R18">
         <v>0</v>
       </c>
-      <c r="S18" t="s">
+      <c r="T18" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>44</v>
       </c>
@@ -1457,7 +1496,7 @@
         <v>0.58299999999999996</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>46</v>
       </c>
@@ -1503,10 +1542,13 @@
         <v>6.7000000000000004E-2</v>
       </c>
       <c r="S20" t="s">
+        <v>90</v>
+      </c>
+      <c r="T20" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>48</v>
       </c>
@@ -1548,8 +1590,11 @@
       <c r="R21">
         <v>0.26200000000000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S21" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>50</v>
       </c>
@@ -1589,7 +1634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>52</v>
       </c>
@@ -1628,7 +1673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>53</v>
       </c>
@@ -1673,8 +1718,11 @@
       <c r="R24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S24" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>58</v>
       </c>
@@ -1706,7 +1754,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>59</v>
       </c>
@@ -1745,7 +1793,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>60</v>
       </c>
@@ -1780,7 +1828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>55</v>
       </c>
@@ -1815,7 +1863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -1850,7 +1898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>57</v>
       </c>
@@ -1890,8 +1938,11 @@
       <c r="R30">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S30" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>81</v>
       </c>
@@ -1926,10 +1977,13 @@
         <v>83</v>
       </c>
       <c r="S31" t="s">
+        <v>89</v>
+      </c>
+      <c r="T31" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>81</v>
       </c>
@@ -1963,11 +2017,14 @@
       <c r="P32" t="s">
         <v>83</v>
       </c>
-      <c r="S32" s="1" t="s">
+      <c r="S32" t="s">
+        <v>89</v>
+      </c>
+      <c r="T32" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>84</v>
       </c>
@@ -2007,11 +2064,14 @@
       <c r="R33">
         <v>0.36</v>
       </c>
-      <c r="S33" s="1" t="s">
+      <c r="S33" t="s">
+        <v>89</v>
+      </c>
+      <c r="T33" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>85</v>
       </c>
@@ -2045,9 +2105,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="S12" r:id="rId1" xr:uid="{DF393319-4305-403F-8ADC-047B02A02027}"/>
-    <hyperlink ref="S32" r:id="rId2" xr:uid="{F8949122-1CA4-4C9A-9926-43CC41147D5D}"/>
-    <hyperlink ref="S33" r:id="rId3" xr:uid="{BFEA82BC-0F1A-4FE2-9C30-7C5358E0CE80}"/>
+    <hyperlink ref="T12" r:id="rId1" xr:uid="{DF393319-4305-403F-8ADC-047B02A02027}"/>
+    <hyperlink ref="T32" r:id="rId2" xr:uid="{F8949122-1CA4-4C9A-9926-43CC41147D5D}"/>
+    <hyperlink ref="T33" r:id="rId3" xr:uid="{BFEA82BC-0F1A-4FE2-9C30-7C5358E0CE80}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>